<commit_message>
Filled in people responsible for each task.
</commit_message>
<xml_diff>
--- a/Sprint Backlog.xlsx
+++ b/Sprint Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Team 47 Sprint Backlog</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>Aziz</t>
+  </si>
+  <si>
+    <t>Mark</t>
   </si>
 </sst>
 </file>
@@ -94,11 +100,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -397,7 +406,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -445,7 +454,10 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D3">
@@ -456,7 +468,10 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D4">
@@ -467,7 +482,10 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D5">

</xml_diff>

<commit_message>
Updated the Sprint Backlog after todays meeting
There was no work done on the actual implementation so all the tasks
remain with the same hours of work left.
</commit_message>
<xml_diff>
--- a/Sprint Backlog.xlsx
+++ b/Sprint Backlog.xlsx
@@ -103,11 +103,11 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -406,7 +406,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -417,15 +417,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
@@ -454,13 +454,16 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
         <v>5</v>
       </c>
     </row>
@@ -468,13 +471,16 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4">
         <v>7</v>
       </c>
     </row>
@@ -482,13 +488,16 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
         <v>10</v>
       </c>
     </row>
@@ -502,7 +511,10 @@
         <f>SUM(D3:D6)</f>
         <v>22</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <f>SUM(E3:E6)</f>
+        <v>22</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>

</xml_diff>